<commit_message>
generated the data for YCbCr color space
</commit_message>
<xml_diff>
--- a/BLACK_SUNRISE_HSV/135_Degree_GLCM/RGB_m.xlsx
+++ b/BLACK_SUNRISE_HSV/135_Degree_GLCM/RGB_m.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4TH YEAR\Project_1\MATRICES_WORKSPACES\BLACK_SUNRISE_HSV\135_Degree_GLCM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3FCA0E-F8B0-4D7C-8417-C92D0538B854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="true"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,16 +51,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,1977 +336,2009 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A400"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.15625" customWidth="true"/>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
     </row>
-    <row r="25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3</v>
       </c>
     </row>
-    <row r="42">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
     </row>
-    <row r="44">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1</v>
       </c>
     </row>
-    <row r="57">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>4</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>4</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>4</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>4</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>4</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>4</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>4</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>4</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>4</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>4</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>3</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>3</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>3</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>3</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>3</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>3</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>3</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>3</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>3</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>1</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>3</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>3</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>3</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>3</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>3</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>3</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>3</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>3</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>3</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>3</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>2</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>3</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>3</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>3</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>3</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>2</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>3</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>3</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>3</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>3</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>3</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>3</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>3</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>3</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>3</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>3</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>3</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>1</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>1</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>1</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>1</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>1</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>1</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>1</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>1</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>1</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>1</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>1</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>1</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>1</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>1</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>1</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>1</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>1</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>1</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>1</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>1</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>2</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>3</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>3</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>3</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>2</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>2</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>2</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>2</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>2</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>2</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>2</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>2</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>2</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>2</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>2</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>2</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>2</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>2</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>3</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>3</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>3</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>2</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>2</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>2</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>2</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>2</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>2</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>2</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>2</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>2</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>2</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>2</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>2</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>2</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>2</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>2</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>2</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>3</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>3</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>3</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>3</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>3</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>3</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>3</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>3</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>1</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>3</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>3</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>3</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>1</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>3</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>3</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>3</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>1</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>3</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>3</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>3</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>3</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>3</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>1</v>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>3</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>2</v>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>1</v>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>1</v>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>1</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>1</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>3</v>
       </c>
     </row>
-    <row r="231">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>3</v>
       </c>
     </row>
-    <row r="232">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>3</v>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>3</v>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>3</v>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>2</v>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>2</v>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>3</v>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>2</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>3</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>3</v>
       </c>
     </row>
-    <row r="241">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>1</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>1</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>1</v>
       </c>
     </row>
-    <row r="244">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>1</v>
       </c>
     </row>
-    <row r="245">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>1</v>
       </c>
     </row>
-    <row r="246">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>1</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>1</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>1</v>
       </c>
     </row>
-    <row r="249">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>1</v>
       </c>
     </row>
-    <row r="250">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>1</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>1</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>1</v>
       </c>
     </row>
-    <row r="253">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>1</v>
       </c>
     </row>
-    <row r="254">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>1</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>1</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>1</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>1</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>1</v>
       </c>
     </row>
-    <row r="259">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>1</v>
       </c>
     </row>
-    <row r="260">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>1</v>
       </c>
     </row>
-    <row r="261">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>1</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>1</v>
       </c>
     </row>
-    <row r="263">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>1</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>1</v>
       </c>
     </row>
-    <row r="265">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>1</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>2</v>
       </c>
     </row>
-    <row r="267">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>1</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>3</v>
       </c>
     </row>
-    <row r="269">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>3</v>
       </c>
     </row>
-    <row r="270">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>3</v>
       </c>
     </row>
-    <row r="271">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>3</v>
       </c>
     </row>
-    <row r="272">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>3</v>
       </c>
     </row>
-    <row r="273">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>3</v>
       </c>
     </row>
-    <row r="274">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>3</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>3</v>
       </c>
     </row>
-    <row r="276">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>3</v>
       </c>
     </row>
-    <row r="277">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>3</v>
       </c>
     </row>
-    <row r="278">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>1</v>
       </c>
     </row>
-    <row r="279">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>1</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>1</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>1</v>
       </c>
     </row>
-    <row r="282">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>1</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>1</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>1</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>1</v>
       </c>
     </row>
-    <row r="286">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>2</v>
       </c>
     </row>
-    <row r="287">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>1</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>3</v>
       </c>
     </row>
-    <row r="289">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>3</v>
       </c>
     </row>
-    <row r="290">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>3</v>
       </c>
     </row>
-    <row r="291">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>3</v>
       </c>
     </row>
-    <row r="292">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>3</v>
       </c>
     </row>
-    <row r="293">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>3</v>
       </c>
     </row>
-    <row r="294">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>3</v>
       </c>
     </row>
-    <row r="295">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>3</v>
       </c>
     </row>
-    <row r="296">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>3</v>
       </c>
     </row>
-    <row r="297">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>3</v>
       </c>
     </row>
-    <row r="298">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>1</v>
       </c>
     </row>
-    <row r="299">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>1</v>
       </c>
     </row>
-    <row r="300">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>1</v>
       </c>
     </row>
-    <row r="301">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>1</v>
       </c>
     </row>
-    <row r="302">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>3</v>
       </c>
     </row>
-    <row r="303">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>4</v>
       </c>
     </row>
-    <row r="304">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>3</v>
       </c>
     </row>
-    <row r="305">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>3</v>
       </c>
     </row>
-    <row r="306">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>3</v>
       </c>
     </row>
-    <row r="307">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>3</v>
       </c>
     </row>
-    <row r="309">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>1</v>
       </c>
     </row>
-    <row r="310">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>3</v>
       </c>
     </row>
-    <row r="311">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>3</v>
       </c>
     </row>
-    <row r="312">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>3</v>
       </c>
     </row>
-    <row r="313">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>3</v>
       </c>
     </row>
-    <row r="314">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>1</v>
       </c>
     </row>
-    <row r="315">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>3</v>
       </c>
     </row>
-    <row r="316">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>3</v>
       </c>
     </row>
-    <row r="317">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>4</v>
       </c>
     </row>
-    <row r="318">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>3</v>
       </c>
     </row>
-    <row r="319">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>3</v>
       </c>
     </row>
-    <row r="320">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>1</v>
       </c>
     </row>
-    <row r="321">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>4</v>
       </c>
     </row>
-    <row r="322">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>2</v>
       </c>
     </row>
-    <row r="323">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>1</v>
       </c>
     </row>
-    <row r="324">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>3</v>
       </c>
     </row>
-    <row r="325">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>3</v>
       </c>
     </row>
-    <row r="326">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>1</v>
       </c>
     </row>
-    <row r="327">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>1</v>
       </c>
     </row>
-    <row r="328">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>1</v>
       </c>
     </row>
-    <row r="329">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>1</v>
       </c>
     </row>
-    <row r="330">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>3</v>
       </c>
     </row>
-    <row r="331">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>3</v>
       </c>
     </row>
-    <row r="332">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>3</v>
       </c>
     </row>
-    <row r="333">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>3</v>
       </c>
     </row>
-    <row r="334">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>2</v>
       </c>
     </row>
-    <row r="335">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>3</v>
       </c>
     </row>
-    <row r="336">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>4</v>
       </c>
     </row>
-    <row r="337">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>4</v>
       </c>
     </row>
-    <row r="338">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>2</v>
       </c>
     </row>
-    <row r="339">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>2</v>
       </c>
     </row>
-    <row r="340">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>3</v>
       </c>
     </row>
-    <row r="341">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>4</v>
       </c>
     </row>
-    <row r="342">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>4</v>
       </c>
     </row>
-    <row r="343">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>4</v>
       </c>
     </row>
-    <row r="344">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>4</v>
       </c>
     </row>
-    <row r="345">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>4</v>
       </c>
     </row>
-    <row r="346">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>1</v>
       </c>
     </row>
-    <row r="347">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>1</v>
       </c>
     </row>
-    <row r="348">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>4</v>
       </c>
     </row>
-    <row r="349">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>1</v>
       </c>
     </row>
-    <row r="350">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>1</v>
       </c>
     </row>
-    <row r="351">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>1</v>
       </c>
     </row>
-    <row r="352">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>1</v>
       </c>
     </row>
-    <row r="353">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>1</v>
       </c>
     </row>
-    <row r="354">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>1</v>
       </c>
     </row>
-    <row r="355">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>1</v>
       </c>
     </row>
-    <row r="356">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>1</v>
       </c>
     </row>
-    <row r="357">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>1</v>
       </c>
     </row>
-    <row r="358">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>1</v>
       </c>
     </row>
-    <row r="359">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>1</v>
       </c>
     </row>
-    <row r="360">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>1</v>
       </c>
     </row>
-    <row r="361">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>4</v>
       </c>
     </row>
-    <row r="362">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>4</v>
       </c>
     </row>
-    <row r="363">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>4</v>
       </c>
     </row>
-    <row r="364">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>4</v>
       </c>
     </row>
-    <row r="365">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>3</v>
       </c>
     </row>
-    <row r="366">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>1</v>
       </c>
     </row>
-    <row r="367">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>4</v>
       </c>
     </row>
-    <row r="368">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>4</v>
       </c>
     </row>
-    <row r="369">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>4</v>
       </c>
     </row>
-    <row r="370">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>4</v>
       </c>
     </row>
-    <row r="371">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>3</v>
       </c>
     </row>
-    <row r="372">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>1</v>
       </c>
     </row>
-    <row r="373">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>1</v>
       </c>
     </row>
-    <row r="374">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>2</v>
       </c>
     </row>
-    <row r="375">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>1</v>
       </c>
     </row>
-    <row r="376">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>2</v>
       </c>
     </row>
-    <row r="377">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>2</v>
       </c>
     </row>
-    <row r="378">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>3</v>
       </c>
     </row>
-    <row r="379">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>3</v>
       </c>
     </row>
-    <row r="380">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>4</v>
       </c>
     </row>
-    <row r="381">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>4</v>
       </c>
     </row>
-    <row r="382">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>4</v>
       </c>
     </row>
-    <row r="383">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>4</v>
       </c>
     </row>
-    <row r="384">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>4</v>
       </c>
     </row>
-    <row r="385">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>3</v>
       </c>
     </row>
-    <row r="386">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>1</v>
       </c>
     </row>
-    <row r="387">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>4</v>
       </c>
     </row>
-    <row r="388">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>4</v>
       </c>
     </row>
-    <row r="389">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>4</v>
       </c>
     </row>
-    <row r="390">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>4</v>
       </c>
     </row>
-    <row r="391">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>3</v>
       </c>
     </row>
-    <row r="392">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>1</v>
       </c>
     </row>
-    <row r="393">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>1</v>
       </c>
     </row>
-    <row r="394">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>2</v>
       </c>
     </row>
-    <row r="395">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>1</v>
       </c>
     </row>
-    <row r="396">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>2</v>
       </c>
     </row>
-    <row r="397">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>2</v>
       </c>
     </row>
-    <row r="398">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>3</v>
       </c>
     </row>
-    <row r="399">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>3</v>
       </c>
     </row>
-    <row r="400">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>4</v>
       </c>

</xml_diff>